<commit_message>
add s3, excel utils
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/test1.xlsx
+++ b/src/test/resources/excel/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASk\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0581A876-9FC9-4EC6-8539-A0A500CD1D2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070FC761-0661-4F9C-B6AA-C4E0E1307C81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8FF55298-434B-4DBE-BA3B-CB61CECEC5C1}"/>
   </bookViews>
@@ -30,77 +30,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>b222</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>c2222</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e222222</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b3333</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>asesdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>e</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>asd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>asdf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>b2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,136 +429,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B8B4A0-E1F8-44E1-AF62-987DF3DF9E24}">
-  <dimension ref="A2:R24"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="K18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="7:18" x14ac:dyDescent="0.3">
-      <c r="R24" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>